<commit_message>
resolved issue with date not excluding time
</commit_message>
<xml_diff>
--- a/init.xlsx
+++ b/init.xlsx
@@ -383,7 +383,7 @@
         </is>
       </c>
       <c r="B2" s="1" t="n">
-        <v>43611</v>
+        <v>43599</v>
       </c>
     </row>
     <row r="3">
@@ -393,7 +393,7 @@
         </is>
       </c>
       <c r="B3" s="1" t="n">
-        <v>43612</v>
+        <v>43600</v>
       </c>
     </row>
     <row r="4">
@@ -403,7 +403,7 @@
         </is>
       </c>
       <c r="B4" s="1" t="n">
-        <v>43613</v>
+        <v>43601</v>
       </c>
     </row>
     <row r="5">
@@ -413,7 +413,7 @@
         </is>
       </c>
       <c r="B5" s="1" t="n">
-        <v>43614</v>
+        <v>43602</v>
       </c>
     </row>
     <row r="6">
@@ -423,7 +423,7 @@
         </is>
       </c>
       <c r="B6" s="1" t="n">
-        <v>43615</v>
+        <v>43603</v>
       </c>
     </row>
     <row r="7">
@@ -433,7 +433,7 @@
         </is>
       </c>
       <c r="B7" s="1" t="n">
-        <v>43616</v>
+        <v>43604</v>
       </c>
     </row>
     <row r="8">
@@ -443,7 +443,7 @@
         </is>
       </c>
       <c r="B8" s="1" t="n">
-        <v>43617</v>
+        <v>43605</v>
       </c>
     </row>
     <row r="9">

</xml_diff>

<commit_message>
cmd shows correct output but file isn't being written
</commit_message>
<xml_diff>
--- a/init.xlsx
+++ b/init.xlsx
@@ -52,11 +52,10 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="21" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -668,12 +667,6 @@
       <c r="B25" s="1" t="n">
         <v>43616</v>
       </c>
-      <c r="C25" s="3" t="n">
-        <v>0.2291666666666667</v>
-      </c>
-      <c r="D25" s="3" t="n">
-        <v>0.40625</v>
-      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">

</xml_diff>